<commit_message>
Fixed ND and BN processing
</commit_message>
<xml_diff>
--- a/EXAMS_INTERNAL/BN/BN-COURSES/N-course-code-creditUnit.xlsx
+++ b/EXAMS_INTERNAL/BN/BN-COURSES/N-course-code-creditUnit.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="320" yWindow="420" windowWidth="18820" windowHeight="6810" activeTab="1"/>
+    <workbookView xWindow="320" yWindow="420" windowWidth="18820" windowHeight="6810" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="N-FIRST-YEAR-FIRST-SEMESTER" sheetId="1" r:id="rId1"/>
@@ -135,51 +135,27 @@
     <t>GNS128</t>
   </si>
   <si>
-    <t>GNS 211</t>
-  </si>
-  <si>
     <t>Anatomy and Physiology III</t>
   </si>
   <si>
-    <t>GNS 212</t>
-  </si>
-  <si>
     <t>Foundation of Nursing III</t>
   </si>
   <si>
-    <t>GNS 213</t>
-  </si>
-  <si>
     <t>Medical-Surgical Nursing II</t>
   </si>
   <si>
-    <t>GNS 214</t>
-  </si>
-  <si>
     <t>Primary Health Care II</t>
   </si>
   <si>
-    <t>GNS 215</t>
-  </si>
-  <si>
     <t>Pharmacology II</t>
   </si>
   <si>
-    <t>GNS 216</t>
-  </si>
-  <si>
     <t>Reproductive Health I</t>
   </si>
   <si>
-    <t>GNS 217</t>
-  </si>
-  <si>
     <t>Research &amp; Statistics I</t>
   </si>
   <si>
-    <t>GNS 218</t>
-  </si>
-  <si>
     <t>Hospital-Based Nursing Practicum II</t>
   </si>
   <si>
@@ -325,6 +301,30 @@
   </si>
   <si>
     <t>GNS324</t>
+  </si>
+  <si>
+    <t>GNS211</t>
+  </si>
+  <si>
+    <t>GNS212</t>
+  </si>
+  <si>
+    <t>GNS213</t>
+  </si>
+  <si>
+    <t>GNS214</t>
+  </si>
+  <si>
+    <t>GNS215</t>
+  </si>
+  <si>
+    <t>GNS216</t>
+  </si>
+  <si>
+    <t>GNS217</t>
+  </si>
+  <si>
+    <t>GNS218</t>
   </si>
 </sst>
 </file>
@@ -799,7 +799,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
@@ -918,8 +918,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -942,10 +942,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B2" t="s">
         <v>37</v>
-      </c>
-      <c r="B2" t="s">
-        <v>38</v>
       </c>
       <c r="C2" s="1">
         <v>3</v>
@@ -953,10 +953,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>39</v>
+        <v>94</v>
       </c>
       <c r="B3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C3" s="1">
         <v>3</v>
@@ -964,10 +964,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>41</v>
+        <v>95</v>
       </c>
       <c r="B4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C4" s="1">
         <v>4</v>
@@ -975,10 +975,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>43</v>
+        <v>96</v>
       </c>
       <c r="B5" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C5" s="1">
         <v>3</v>
@@ -986,10 +986,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>45</v>
+        <v>97</v>
       </c>
       <c r="B6" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C6" s="1">
         <v>2</v>
@@ -997,10 +997,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>47</v>
+        <v>98</v>
       </c>
       <c r="B7" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C7" s="1">
         <v>3</v>
@@ -1008,10 +1008,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>49</v>
+        <v>99</v>
       </c>
       <c r="B8" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="C8" s="1">
         <v>2</v>
@@ -1019,10 +1019,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>51</v>
+        <v>100</v>
       </c>
       <c r="B9" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="C9" s="1">
         <v>4</v>
@@ -1061,10 +1061,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="B2" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="C2" s="1">
         <v>3</v>
@@ -1072,10 +1072,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="B3" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="C3" s="1">
         <v>4</v>
@@ -1083,10 +1083,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="B4" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="C4" s="1">
         <v>2</v>
@@ -1094,10 +1094,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="B5" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="C5" s="1">
         <v>2</v>
@@ -1105,10 +1105,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="B6" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="C6" s="1">
         <v>2</v>
@@ -1116,10 +1116,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="B7" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="C7" s="1">
         <v>3</v>
@@ -1127,10 +1127,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="B8" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="C8" s="1">
         <v>2</v>
@@ -1138,10 +1138,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="B9" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="C9" s="1">
         <v>4</v>
@@ -1149,10 +1149,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="B10" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="C10" s="1">
         <v>2</v>
@@ -1191,10 +1191,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="B2" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="C2" s="1">
         <v>3</v>
@@ -1202,10 +1202,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="B3" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C3" s="1">
         <v>2</v>
@@ -1213,10 +1213,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="B4" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="C4" s="1">
         <v>2</v>
@@ -1224,10 +1224,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="B5" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="C5" s="1">
         <v>3</v>
@@ -1235,10 +1235,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="B6" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="C6" s="1">
         <v>3</v>
@@ -1246,10 +1246,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="B7" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="C7" s="1">
         <v>3</v>
@@ -1257,10 +1257,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="B8" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="C8" s="1">
         <v>2</v>
@@ -1268,10 +1268,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="B9" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C9" s="1">
         <v>4</v>
@@ -1310,10 +1310,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="B2" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="C2" s="1">
         <v>3</v>
@@ -1321,10 +1321,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="B3" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="C3" s="1">
         <v>3</v>
@@ -1332,10 +1332,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="B4" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="C4" s="1">
         <v>2</v>
@@ -1343,10 +1343,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="B5" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="C5" s="1">
         <v>3</v>
@@ -1354,10 +1354,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="B6" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="C6" s="1">
         <v>2</v>
@@ -1365,10 +1365,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="B7" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="C7" s="1">
         <v>3</v>
@@ -1376,10 +1376,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="B8" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="C8" s="1">
         <v>4</v>

</xml_diff>